<commit_message>
bf: add tas forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2023/july/bf_lf_tas1_202306_2_participant.xlsx
+++ b/LF/TAS/Burkina Faso/2023/july/bf_lf_tas1_202306_2_participant.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\LF\TAS\Burkina Faso\2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2023\july\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DB2B00-6B74-4916-9FC2-2A1370624B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2662DEA-FF84-458B-8E3F-9E4C2B92F547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -307,12 +307,6 @@
     <t>p_nom_CSPS</t>
   </si>
   <si>
-    <t>(Avril 2023) Burkina Faso TAS FL - 2. Formulaire Enrôlement V2.2</t>
-  </si>
-  <si>
-    <t>bf_lf_tas1_202304_2_participant_v2_2</t>
-  </si>
-  <si>
     <t>. &gt;=5 and . &lt;=10</t>
   </si>
   <si>
@@ -329,6 +323,12 @@
   </si>
   <si>
     <t>10 ans</t>
+  </si>
+  <si>
+    <t>bf_lf_tas1_202306_2_participant</t>
+  </si>
+  <si>
+    <t>(Juillet 2023) Burkina Faso TAS FL - 2. Formulaire Enrôlement</t>
   </si>
 </sst>
 </file>
@@ -1122,10 +1122,10 @@
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="7" t="s">
@@ -1219,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -1395,7 +1395,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D16" s="14"/>
     </row>
@@ -1431,7 +1431,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D19" s="14"/>
     </row>
@@ -1443,7 +1443,7 @@
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D20" s="14"/>
     </row>
@@ -1455,7 +1455,7 @@
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D21" s="14"/>
     </row>
@@ -1662,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1688,10 +1688,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>41</v>

</xml_diff>